<commit_message>
Fixed trouble with output file
</commit_message>
<xml_diff>
--- a/src/main/resources/wordAndExcelTemplates/Пример таблицы.xlsx
+++ b/src/main/resources/wordAndExcelTemplates/Пример таблицы.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\universityProject\UniversityProject\src\main\resources\wordAndExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEE367D-E98C-45C9-AA52-BD037B1FECF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4064A1-8649-4CF5-8B23-1D48994F07E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1623716-4A27-4E1C-BCF6-4F3F7F47B2DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>Синицын Тимофей Евгеньевич</t>
   </si>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C79337-56E6-4364-9187-2AC508AECDA0}">
-  <dimension ref="A2:B30"/>
+  <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,158 +481,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>